<commit_message>
update generic profiles (#276)
* update generic profiles

* Update input/fsh/profiles/AsPersonProfile.fsh

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* Update input/fsh/profiles/AsPractitionerProfile.fsh

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* Update input/fsh/profiles/AsPersonProfile.fsh

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* Update input/fsh/profiles/AsOrganizationProfile.fsh

Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com>

* Update AsPersonProfile.fsh

---------

Co-authored-by: William AZIS <william.azis@esante.gouv.fr>
Co-authored-by: Nicolas Riss <48218773+nriss@users.noreply.github.com> f5e165a7964ab78e614b6e9677139998d387bc09
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-as-address-extended.xlsx
+++ b/main/ig/StructureDefinition-as-address-extended.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-18T15:54:11+00:00</t>
+    <t>2025-10-08T12:14:02+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -4212,7 +4212,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
         <v>249</v>
       </c>
@@ -4557,7 +4557,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="29" hidden="true">
+    <row r="29">
       <c r="A29" t="s" s="2">
         <v>276</v>
       </c>
@@ -4791,12 +4791,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AO30">
-    <filterColumn colId="6">
+    <filterColumn colId="7">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <filterColumn colId="26">
+    <filterColumn colId="27">
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>

</xml_diff>